<commit_message>
Saldo contas feito até a calculadora da edição da carteira
</commit_message>
<xml_diff>
--- a/src/main/resources/massa.xlsx
+++ b/src/main/resources/massa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SempreIT\Desktop\smiles-automation-qa-app_android\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SempreIT\Documents\app_fortuno\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>REG</t>
   </si>
   <si>
-    <t>in_alguma_coisa</t>
+    <t>REG-101</t>
   </si>
   <si>
-    <t>REG-101</t>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>in_Saldo_Da_Conta</t>
   </si>
 </sst>
 </file>
@@ -68,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,26 +354,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finalização calc e adição na massa
</commit_message>
<xml_diff>
--- a/src/main/resources/massa.xlsx
+++ b/src/main/resources/massa.xlsx
@@ -81,16 +81,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,11 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -405,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,14 +465,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="3"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reg 302 e 303 terminadas
</commit_message>
<xml_diff>
--- a/src/main/resources/massa.xlsx
+++ b/src/main/resources/massa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pietr\Documents\Auto\app_fortuno\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SempreIT\Documents\app_fortuno\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>REG</t>
   </si>
@@ -75,14 +75,43 @@
   </si>
   <si>
     <t>in_Valor_Calculadora_Transferencia</t>
+  </si>
+  <si>
+    <t>REG-402</t>
+  </si>
+  <si>
+    <t>3250000</t>
+  </si>
+  <si>
+    <t>in_Quantidade_Parcelas</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>REG-403</t>
+  </si>
+  <si>
+    <t>6963455</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,12 +139,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,9 +442,10 @@
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +470,11 @@
       <c r="H1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -447,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -464,7 +499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -478,6 +513,34 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
orçamento finalizado, perfil ajuste finalizado,total geral finalizado, cartões de crédito em andamento
</commit_message>
<xml_diff>
--- a/src/main/resources/massa.xlsx
+++ b/src/main/resources/massa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>REG</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>REG-501</t>
+  </si>
+  <si>
+    <t>23243543</t>
+  </si>
+  <si>
+    <t>REG-202</t>
+  </si>
+  <si>
+    <t>232435343</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>REG-203</t>
+  </si>
+  <si>
+    <t>2232444</t>
   </si>
 </sst>
 </file>
@@ -436,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,8 +530,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
+      <c r="A4" t="s">
+        <v>29</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -518,48 +539,76 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
+      <c r="A5" t="s">
+        <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H9" s="5"/>
-    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REG 205 COM ERRO
</commit_message>
<xml_diff>
--- a/src/main/resources/massa.xlsx
+++ b/src/main/resources/massa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>REG</t>
   </si>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t>2232444</t>
+  </si>
+  <si>
+    <t>REG-204</t>
+  </si>
+  <si>
+    <t>324234543</t>
+  </si>
+  <si>
+    <t>REG-206</t>
+  </si>
+  <si>
+    <t>in_Confirmar_Exclusao</t>
+  </si>
+  <si>
+    <t>Confirmar</t>
   </si>
 </sst>
 </file>
@@ -457,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,9 +488,10 @@
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,8 +519,11 @@
       <c r="I1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -512,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -529,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -546,7 +565,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -554,60 +573,76 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="H10" s="1" t="s">
+      <c r="C12" s="5"/>
+      <c r="H12" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G14" s="5"/>
     </row>
   </sheetData>

</xml_diff>